<commit_message>
regen: get rid of duplicate field / link: wrap line
</commit_message>
<xml_diff>
--- a/docs/sample-block/sample-block.xlsx
+++ b/docs/sample-block/sample-block.xlsx
@@ -168,7 +168,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If surgical sample, how far from the pathology was the sample obtained. Typically a number of centimeters. Leave blank if not applicable or unknown.</t>
+          <t>The media used during preparation of the sample.</t>
         </r>
       </text>
     </comment>
@@ -181,7 +181,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The media used during preparation of the sample.</t>
+          <t>The temperature for the preparation process.</t>
         </r>
       </text>
     </comment>
@@ -194,7 +194,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The temperature for the preparation process.</t>
+          <t>The amount of time that elapsed from beginning of sampling to the first preservation (time from when received in lab to preservation). This would, for example, represent how long it took to cut the tissue and freeze it.</t>
         </r>
       </text>
     </comment>
@@ -207,7 +207,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The amount of time that elapsed from beginning of sampling to the first preservation (time from when received in lab to preservation). This would, for example, represent how long it took to cut the tissue and freeze it.</t>
+          <t>Time unit</t>
         </r>
       </text>
     </comment>
@@ -220,7 +220,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time unit</t>
+          <t>What was the sample preserved in.</t>
         </r>
       </text>
     </comment>
@@ -233,7 +233,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>What was the sample preserved in.</t>
+          <t>The temperature during storage, after preparation and before the assay is performed.</t>
         </r>
       </text>
     </comment>
@@ -246,7 +246,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The temperature during storage, after preparation and before the assay is performed.</t>
+          <t>For example, RIN: 8.7. For suspensions, measured by visual inspection prior to cell lysis or defined by known parameters such as wells with several cells or no cells. This can be captured at a high level. "OK" or "not OK", or with more specificity such as "debris", "clump", "low clump".</t>
         </r>
       </text>
     </comment>
@@ -259,24 +259,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>For example, RIN: 8.7. For suspensions, measured by visual inspection prior to cell lysis or defined by known parameters such as wells with several cells or no cells. This can be captured at a high level. "OK" or "not OK", or with more specificity such as "debris", "clump", "low clump".</t>
+          <t>histopathological reporting of key variables that are important for the tissue (absence of necrosis, comment on composition, significant pathology description, high level inflammation/fibrosis assessment etc</t>
         </r>
       </text>
     </comment>
     <comment ref="S1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>histopathological reporting of key variables that are important for the tissue (absence of necrosis, comment on composition, significant pathology description, high level inflammation/fibrosis assessment etc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -294,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t>version</t>
   </si>
@@ -852,7 +839,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -861,7 +848,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,38 +880,35 @@
         <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" s="1" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="16">
+  <dataValidations count="15">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -956,27 +940,23 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="K2:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from preparation_media list." sqref="K2:K1048576">
+      <formula1>'preparation_media list'!$A$1:$A$14</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from preparation_temperature list." sqref="L2:L1048576">
+      <formula1>'preparation_temperature list'!$A$1:$A$8</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="M2:M1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from preparation_media list." sqref="L2:L1048576">
-      <formula1>'preparation_media list'!$A$1:$A$14</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from preparation_temperature list." sqref="M2:M1048576">
-      <formula1>'preparation_temperature list'!$A$1:$A$8</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="N2:N1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: min / hours / days." sqref="O2:O1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: min / hours / days." sqref="N2:N1048576">
       <formula1>'processing_time_unit list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from storage_media list." sqref="P2:P1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from storage_media list." sqref="O2:O1048576">
       <formula1>'storage_media list'!$A$1:$A$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from storage_temperature list." sqref="Q2:Q1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from storage_temperature list." sqref="P2:P1048576">
       <formula1>'storage_temperature list'!$A$1:$A$12</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>